<commit_message>
Corrections and Additions in Italian UI (it.json) (#1530)
* Add files via upload

* Add files via upload

* Add files via upload

* Add files via upload

* Add files via upload

* Add files via upload

* Update it.json

Update Italian language

* Update it.json

Added the missing lines and adjusted a section that was translated literally to make it more natural and accurate.

* Update it.json

Updated little adjustments.
</commit_message>
<xml_diff>
--- a/tools/matrix/risk-matrix-5x5-iso-27005.xlsx
+++ b/tools/matrix/risk-matrix-5x5-iso-27005.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/matrix/5x5-iso-27005/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovanni/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB147526-EDEF-B845-8D10-0693FF792B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27FBAFC-A0E2-3F4F-BFF3-F593C63AE0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="20300" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33360" windowHeight="20300" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="144">
   <si>
     <t>library_urn</t>
   </si>
@@ -358,18 +358,135 @@
   </si>
   <si>
     <t>1 - improbable</t>
+  </si>
+  <si>
+    <t>name[it]</t>
+  </si>
+  <si>
+    <t>description[it]</t>
+  </si>
+  <si>
+    <t>5 - quasi certo</t>
+  </si>
+  <si>
+    <t>La verosimiglianza dello scenario di rischio è molto alta</t>
+  </si>
+  <si>
+    <t>4 - molto probabile</t>
+  </si>
+  <si>
+    <t>La verosimiglianza dello scenario di rischio è alta</t>
+  </si>
+  <si>
+    <t>3 - probabile</t>
+  </si>
+  <si>
+    <t>La verosimiglianza dello scenario di rischio è significativa</t>
+  </si>
+  <si>
+    <t>2 - piuttosto improbabile</t>
+  </si>
+  <si>
+    <t>La verosimiglianza dello scenario di rischio è bassa</t>
+  </si>
+  <si>
+    <t>1 - improbabile</t>
+  </si>
+  <si>
+    <t>La verosimiglianza dello scenario di rischio è molto bassa</t>
+  </si>
+  <si>
+    <t>1 - minore</t>
+  </si>
+  <si>
+    <t>Conseguenze trascurabili per l'organizzazione</t>
+  </si>
+  <si>
+    <t>2 - significativo</t>
+  </si>
+  <si>
+    <t>Conseguenze significative ma limitate per l'organizzazione</t>
+  </si>
+  <si>
+    <t>3 - serio</t>
+  </si>
+  <si>
+    <t>Conseguenze sostanziali per l'organizzazione</t>
+  </si>
+  <si>
+    <t>4 - critico</t>
+  </si>
+  <si>
+    <t>Conseguenze disastrose per l'organizzazione</t>
+  </si>
+  <si>
+    <t>5 - catastrofico</t>
+  </si>
+  <si>
+    <t>Conseguenze settoriali o regolamentari oltre l'organizzazione</t>
+  </si>
+  <si>
+    <t>1 - molto basso</t>
+  </si>
+  <si>
+    <t>molto basso - rischio accettabile</t>
+  </si>
+  <si>
+    <t>2 - basso</t>
+  </si>
+  <si>
+    <t>basso - rischio accettabile</t>
+  </si>
+  <si>
+    <t>3 - medio</t>
+  </si>
+  <si>
+    <t>medio - rischio tollerabile</t>
+  </si>
+  <si>
+    <t>4 - alto</t>
+  </si>
+  <si>
+    <t>alto - rischio inaccettabile</t>
+  </si>
+  <si>
+    <t>5 - molto alto</t>
+  </si>
+  <si>
+    <t>molto alto - rischio inaccettabile</t>
+  </si>
+  <si>
+    <t>library_name[it]</t>
+  </si>
+  <si>
+    <t>library_description[it]</t>
+  </si>
+  <si>
+    <t>Matrice 5x5 descritta nella norma ISO-27005 allegato A</t>
+  </si>
+  <si>
+    <t>risk_matrix_name[it]</t>
+  </si>
+  <si>
+    <t>risk_matrix_description[it]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -501,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -564,9 +681,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -593,7 +711,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -909,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF47FB7-BAFE-4E46-A187-08E7F45C581C}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -935,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1067,6 +1185,38 @@
       </c>
       <c r="B18" s="1" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1077,10 +1227,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C78439-E0E8-6B46-8D3C-6DE0FA8D6D39}">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1092,10 +1242,12 @@
     <col min="6" max="6" width="49.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="10.83203125" style="2"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="59.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="51.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1135,8 +1287,14 @@
       <c r="M1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1173,8 +1331,14 @@
       <c r="M2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1211,8 +1375,14 @@
       <c r="M3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="O3" s="22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1249,8 +1419,14 @@
       <c r="M4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="O4" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1287,8 +1463,14 @@
       <c r="M5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="O5" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1325,8 +1507,14 @@
       <c r="M6" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="O6" s="22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1348,8 +1536,14 @@
       <c r="M7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="O7" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1371,8 +1565,14 @@
       <c r="M8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="O8" s="22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1394,8 +1594,14 @@
       <c r="M9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1417,8 +1623,14 @@
       <c r="M10" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1440,8 +1652,14 @@
       <c r="M11" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="O11" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1464,8 +1682,14 @@
       <c r="M12" s="7" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="O12" s="22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1488,8 +1712,14 @@
       <c r="M13" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="O13" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1512,8 +1742,14 @@
       <c r="M14" s="9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="O14" s="22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1536,8 +1772,14 @@
       <c r="M15" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="O15" s="22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1559,6 +1801,12 @@
       </c>
       <c r="M16" s="1" t="s">
         <v>94</v>
+      </c>
+      <c r="N16" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="O16" s="22" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>